<commit_message>
edit docs and examples
</commit_message>
<xml_diff>
--- a/examples/report.xlsx
+++ b/examples/report.xlsx
@@ -15,18 +15,18 @@
     <sheet name="Сводная" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Активности!$A$8:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Активности!$A$7:$B$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Медиа!$A$1:$B$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Молчуны!$A$1:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Сводная!$A$4:$D$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Топы!$A$1:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Молчуны!$A$1:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Сводная!$A$4:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Топы!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
   <si>
     <t>Дни</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Итог по участникам</t>
   </si>
   <si>
-    <t>UserHash</t>
+    <t>FromID</t>
   </si>
   <si>
     <t>Имя</t>
@@ -67,22 +67,16 @@
     <t>M</t>
   </si>
   <si>
-    <t>afecc820c7</t>
-  </si>
-  <si>
-    <t>7705dc6af6</t>
-  </si>
-  <si>
-    <t>90b43dbac6</t>
-  </si>
-  <si>
-    <t>АДМИН</t>
-  </si>
-  <si>
-    <t>УЧАСТНИК3</t>
-  </si>
-  <si>
-    <t>УЧАСТНИК2</t>
+    <t>userA123456789</t>
+  </si>
+  <si>
+    <t>userB987654321</t>
+  </si>
+  <si>
+    <t>Пользователь A</t>
+  </si>
+  <si>
+    <t>Пользователь B</t>
   </si>
   <si>
     <t>Помесячно (длинная)</t>
@@ -91,7 +85,7 @@
     <t>Месяц</t>
   </si>
   <si>
-    <t>2024-10</t>
+    <t>2025-10</t>
   </si>
   <si>
     <t>Кросс-таблица (участник × месяц)</t>
@@ -151,25 +145,25 @@
     <t>Имя входного файла</t>
   </si>
   <si>
-    <t>raw[0].json</t>
+    <t>example[0].json</t>
   </si>
   <si>
     <t>Дата/время генерации</t>
   </si>
   <si>
-    <t>2025-11-17 14:30:51</t>
+    <t>2025-12-06 17:17:53</t>
   </si>
   <si>
     <t>Часовой пояс</t>
   </si>
   <si>
-    <t>Созданы поля 'meta_norm' с примененным сдвигом -5</t>
+    <t>Созданы поля 'meta_norm' с примененным сдвигом +5</t>
   </si>
   <si>
     <t>Период (Созданы)</t>
   </si>
   <si>
-    <t>2024-10-04 — 2024-10-05</t>
+    <t>2025-10-18 — 2025-10-18</t>
   </si>
   <si>
     <t>Итоги по чату</t>
@@ -208,7 +202,7 @@
     <t>Отсутствующая/невалидная дата</t>
   </si>
   <si>
-    <t>Пустой/некорректный user_hash</t>
+    <t>Пустой/некорректный from_id</t>
   </si>
   <si>
     <t>Данные для создания сводной таблицы</t>
@@ -229,7 +223,7 @@
     <t>3. Настройте поля:</t>
   </si>
   <si>
-    <t xml:space="preserve">   - Строки: UserHash, Имя</t>
+    <t xml:space="preserve">   - Строки: FromID, Имя</t>
   </si>
   <si>
     <t xml:space="preserve">   - Столбцы: Месяц</t>
@@ -632,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -660,36 +654,36 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5">
-        <v>45569</v>
+        <v>45948</v>
       </c>
       <c r="B3" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="5">
-        <v>45570</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -697,7 +691,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -705,23 +699,23 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -729,7 +723,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -737,7 +731,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -745,7 +739,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -753,7 +747,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -761,7 +755,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -769,7 +763,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
@@ -777,7 +771,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -785,7 +779,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -793,7 +787,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -801,7 +795,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -809,15 +803,15 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -825,7 +819,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -833,7 +827,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -841,7 +835,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -849,7 +843,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -857,7 +851,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -865,23 +859,15 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1">
-        <v>23</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A8:B32"/>
-  <conditionalFormatting sqref="B3:B4">
+  <autoFilter ref="A7:B31"/>
+  <conditionalFormatting sqref="B3">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min" val="0"/>
@@ -890,7 +876,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B32">
+  <conditionalFormatting sqref="B8:B31">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min" val="0"/>
@@ -905,7 +891,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -958,16 +944,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>10.5</v>
+        <v>49</v>
       </c>
       <c r="E3">
-        <v>45.66</v>
+        <v>213.06</v>
       </c>
       <c r="F3" s="6">
         <v>0</v>
@@ -984,181 +970,127 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>152.19</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="E4">
-        <v>15.22</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="E5">
-        <v>15.22</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="2">
         <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E19"/>
-  <conditionalFormatting sqref="C3:C5">
+  <autoFilter ref="A1:E16"/>
+  <conditionalFormatting sqref="C3:C4">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min" val="0"/>
@@ -1167,7 +1099,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D19">
+  <conditionalFormatting sqref="D15:D16">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min" val="0"/>
@@ -1191,8 +1123,8 @@
           <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Топы'!C19:C19</xm:f>
-              <xm:sqref>E19</xm:sqref>
+              <xm:f>'Топы'!C16:C16</xm:f>
+              <xm:sqref>E16</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1207,24 +1139,8 @@
           <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Топы'!C18:C18</xm:f>
-              <xm:sqref>E18</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
-          <x14:colorNegative theme="5"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="4"/>
-          <x14:colorLow theme="4"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Топы'!C17:C17</xm:f>
-              <xm:sqref>E17</xm:sqref>
+              <xm:f>'Топы'!C15:C15</xm:f>
+              <xm:sqref>E15</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1248,7 +1164,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1256,15 +1172,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -1272,7 +1188,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -1280,7 +1196,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -1288,7 +1204,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1296,7 +1212,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1304,7 +1220,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -1312,7 +1228,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1320,7 +1236,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1328,7 +1244,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1336,7 +1252,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1344,7 +1260,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1352,7 +1268,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -1375,7 +1291,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1402,36 +1318,25 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
       <c r="C3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C4"/>
+  <autoFilter ref="A1:C3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1449,115 +1354,115 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13">
-        <v>0.06570841889117043</v>
+        <v>0.03285420944558522</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="7" customFormat="1">
       <c r="A18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
@@ -1565,7 +1470,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -1587,7 +1492,7 @@
           <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Активности'!B3:B4</xm:f>
+              <xm:f>'Активности'!B3:B3</xm:f>
               <xm:sqref>B15</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
@@ -1600,7 +1505,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1614,17 +1519,17 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>6</v>
@@ -1638,7 +1543,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -1652,88 +1557,74 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="9" t="s">
-        <v>63</v>
+      <c r="A10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:D7"/>
+  <autoFilter ref="A4:D6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>